<commit_message>
chgt noms images masques
</commit_message>
<xml_diff>
--- a/images/test.xlsx
+++ b/images/test.xlsx
@@ -438,7 +438,7 @@
         </is>
       </c>
       <c r="F1" t="n">
-        <v>0</v>
+        <v>1.685193628587822</v>
       </c>
       <c r="G1" t="inlineStr">
         <is>
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="H1" t="n">
-        <v>0</v>
+        <v>0.7395101602815672</v>
       </c>
     </row>
     <row r="2">
@@ -458,64 +458,64 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>moy transgression</t>
+          <t>moyenne hantel</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.436885088002929</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>E-T transgression</t>
+          <t>E-T hantel</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>0.5338222578240785</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>1.847422334842916</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1.16521230467429</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>2.280350850198276</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1.060954090791133</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>1.958717916262161</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1.064737449050925</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0</v>
+        <v>1.675774202594786</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>0.9540319654762321</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>1.893308053280127</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1.157495537083123</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0</v>
+        <v>2.12184406171194</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -523,7 +523,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>1.788854381999832</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -531,15 +531,15 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0</v>
+        <v>1.629643428765334</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>0.7139598849653022</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>2.252370025485892</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -555,7 +555,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0</v>
+        <v>2.100114365777487</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0</v>
+        <v>1.969966809560311</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>2.07434436975044</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>

</xml_diff>